<commit_message>
travail sur le cahier des charges
</commit_message>
<xml_diff>
--- a/Autres/Projet 3 - Gantt.xlsx
+++ b/Autres/Projet 3 - Gantt.xlsx
@@ -102,9 +102,6 @@
     <t>Maquettes haute qualité</t>
   </si>
   <si>
-    <t>Page d'aacueil - blog</t>
-  </si>
-  <si>
     <t>Page films + module fils projetés</t>
   </si>
   <si>
@@ -124,6 +121,9 @@
   </si>
   <si>
     <t>Rédaction document utilisation</t>
+  </si>
+  <si>
+    <t>Page d'acueil - blog</t>
   </si>
 </sst>
 </file>
@@ -624,8 +624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M20" sqref="L20:M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -754,12 +754,8 @@
       <c r="A5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="8">
-        <v>43346</v>
-      </c>
-      <c r="C5" s="8">
-        <v>43199</v>
-      </c>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
       <c r="D5" s="9">
         <f>SUM(D6:D10)</f>
         <v>3.5</v>
@@ -971,7 +967,7 @@
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="35" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B18" s="37">
         <v>43209</v>
@@ -1020,7 +1016,7 @@
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" s="36" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="B21" s="32">
         <v>43220</v>
@@ -1037,7 +1033,7 @@
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" s="36" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B22" s="32">
         <v>43224</v>
@@ -1054,7 +1050,7 @@
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" s="36" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B23" s="32">
         <v>43229</v>
@@ -1071,7 +1067,7 @@
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" s="36" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B24" s="32">
         <v>43235</v>
@@ -1088,7 +1084,7 @@
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" s="36" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B25" s="32">
         <v>43236</v>
@@ -1105,7 +1101,7 @@
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" s="36" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B26" s="32">
         <v>43237</v>
@@ -1120,7 +1116,7 @@
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="35" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B27" s="11">
         <v>43238</v>

</xml_diff>